<commit_message>
removed championship type IWF as it doesn't matter.
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/DE-AgeGroups_de.xlsx
+++ b/owlcms/src/main/resources/agegroups/DE-AgeGroups_de.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABEE59E-AEEF-4A46-8101-01C4A6EB49C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="2640" yWindow="2925" windowWidth="23985" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BW vs AgeGroups" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="BW vs AgeGroups" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -20,293 +34,267 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="78">
-  <si>
-    <t xml:space="preserve">code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">championship Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#bodyweight categories or each age group (bodyweight category code followed by optional qualifying total, example: 45 80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MASTERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IWF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFAULT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M49</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="77">
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>championship Name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>#bodyweight categories or each age group (bodyweight category code followed by optional qualifying total, example: 45 80)</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>F999</t>
+  </si>
+  <si>
+    <t>U13</t>
+  </si>
+  <si>
+    <t>F40</t>
+  </si>
+  <si>
+    <t>F44</t>
+  </si>
+  <si>
+    <t>F48</t>
+  </si>
+  <si>
+    <t>F53</t>
+  </si>
+  <si>
+    <t>F58</t>
+  </si>
+  <si>
+    <t>F63</t>
+  </si>
+  <si>
+    <t>U15</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>F69</t>
+  </si>
+  <si>
+    <t>F75</t>
+  </si>
+  <si>
+    <t>U20</t>
+  </si>
+  <si>
+    <t>F45</t>
+  </si>
+  <si>
+    <t>F49</t>
+  </si>
+  <si>
+    <t>F55</t>
+  </si>
+  <si>
+    <t>F59</t>
+  </si>
+  <si>
+    <t>F64</t>
+  </si>
+  <si>
+    <t>F71</t>
+  </si>
+  <si>
+    <t>F76</t>
+  </si>
+  <si>
+    <t>F81</t>
+  </si>
+  <si>
+    <t>F87</t>
+  </si>
+  <si>
+    <t>U23</t>
+  </si>
+  <si>
+    <t>O21</t>
+  </si>
+  <si>
+    <t>F30</t>
+  </si>
+  <si>
+    <t>MASTERS</t>
+  </si>
+  <si>
+    <t>F35</t>
+  </si>
+  <si>
+    <t>F50</t>
+  </si>
+  <si>
+    <t>F60</t>
+  </si>
+  <si>
+    <t>F65</t>
+  </si>
+  <si>
+    <t>F70</t>
+  </si>
+  <si>
+    <t>F80</t>
+  </si>
+  <si>
+    <t>F85</t>
+  </si>
+  <si>
+    <t>YTH</t>
+  </si>
+  <si>
+    <t>JR</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>M999</t>
+  </si>
+  <si>
+    <t>M35</t>
+  </si>
+  <si>
+    <t>M40</t>
+  </si>
+  <si>
+    <t>M45</t>
+  </si>
+  <si>
+    <t>M50</t>
+  </si>
+  <si>
+    <t>M56</t>
+  </si>
+  <si>
+    <t>M62</t>
+  </si>
+  <si>
+    <t>M69</t>
+  </si>
+  <si>
+    <t>M77</t>
+  </si>
+  <si>
+    <t>M85</t>
+  </si>
+  <si>
+    <t>M94</t>
+  </si>
+  <si>
+    <t>M55</t>
+  </si>
+  <si>
+    <t>M61</t>
+  </si>
+  <si>
+    <t>M67</t>
+  </si>
+  <si>
+    <t>M73</t>
+  </si>
+  <si>
+    <t>M81</t>
+  </si>
+  <si>
+    <t>M89</t>
+  </si>
+  <si>
+    <t>M96</t>
+  </si>
+  <si>
+    <t>M102</t>
+  </si>
+  <si>
+    <t>M109</t>
+  </si>
+  <si>
+    <t>M30</t>
+  </si>
+  <si>
+    <t>M60</t>
+  </si>
+  <si>
+    <t>M65</t>
+  </si>
+  <si>
+    <t>M70</t>
+  </si>
+  <si>
+    <t>M75</t>
+  </si>
+  <si>
+    <t>M80</t>
+  </si>
+  <si>
+    <t>M49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -325,7 +313,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -333,73 +321,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -458,60 +400,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -543,7 +501,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -567,7 +525,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -627,31 +585,30 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.86"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -673,24 +630,24 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+    </row>
+    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -703,14 +660,14 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="n">
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
         <v>10</v>
       </c>
-      <c r="G2" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G2" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -730,7 +687,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -743,14 +700,14 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="5">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="5">
         <v>13</v>
       </c>
-      <c r="G3" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G3" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H3" s="2"/>
@@ -782,7 +739,7 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -795,14 +752,14 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="5">
         <v>14</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="5">
         <v>15</v>
       </c>
-      <c r="G4" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G4" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H4" s="2"/>
@@ -834,7 +791,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -847,14 +804,14 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="5">
         <v>16</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="5">
         <v>17</v>
       </c>
-      <c r="G5" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G5" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H5" s="2"/>
@@ -888,7 +845,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -901,14 +858,14 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="5">
         <v>18</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="5">
         <v>20</v>
       </c>
-      <c r="G6" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G6" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H6" s="2"/>
@@ -948,7 +905,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -961,14 +918,14 @@
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="5">
         <v>18</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="5">
         <v>23</v>
       </c>
-      <c r="G7" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G7" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="2"/>
@@ -1008,7 +965,7 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -1021,14 +978,14 @@
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="5">
         <v>21</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="5">
         <v>999</v>
       </c>
-      <c r="G8" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G8" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H8" s="2"/>
@@ -1068,7 +1025,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1081,14 +1038,14 @@
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="5">
         <v>30</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="5">
         <v>34</v>
       </c>
-      <c r="G9" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G9" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H9" s="2"/>
@@ -1128,7 +1085,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -1141,14 +1098,14 @@
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="5">
         <v>35</v>
       </c>
-      <c r="F10" s="6" t="n">
+      <c r="F10" s="5">
         <v>39</v>
       </c>
-      <c r="G10" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G10" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H10" s="2"/>
@@ -1188,7 +1145,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1201,14 +1158,14 @@
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="5">
         <v>40</v>
       </c>
-      <c r="F11" s="6" t="n">
+      <c r="F11" s="5">
         <v>44</v>
       </c>
-      <c r="G11" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G11" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H11" s="2"/>
@@ -1248,7 +1205,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1261,14 +1218,14 @@
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="6" t="n">
+      <c r="E12" s="5">
         <v>45</v>
       </c>
-      <c r="F12" s="6" t="n">
+      <c r="F12" s="5">
         <v>49</v>
       </c>
-      <c r="G12" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G12" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H12" s="2"/>
@@ -1308,7 +1265,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1321,14 +1278,14 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="5">
         <v>50</v>
       </c>
-      <c r="F13" s="6" t="n">
+      <c r="F13" s="5">
         <v>54</v>
       </c>
-      <c r="G13" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G13" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H13" s="2"/>
@@ -1368,7 +1325,7 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1381,14 +1338,14 @@
       <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="6" t="n">
+      <c r="E14" s="5">
         <v>55</v>
       </c>
-      <c r="F14" s="6" t="n">
+      <c r="F14" s="5">
         <v>59</v>
       </c>
-      <c r="G14" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G14" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H14" s="2"/>
@@ -1428,7 +1385,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1441,14 +1398,14 @@
       <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="6" t="n">
+      <c r="E15" s="5">
         <v>60</v>
       </c>
-      <c r="F15" s="6" t="n">
+      <c r="F15" s="5">
         <v>64</v>
       </c>
-      <c r="G15" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G15" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H15" s="2"/>
@@ -1488,7 +1445,7 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1501,14 +1458,14 @@
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="6" t="n">
+      <c r="E16" s="5">
         <v>65</v>
       </c>
-      <c r="F16" s="6" t="n">
+      <c r="F16" s="5">
         <v>69</v>
       </c>
-      <c r="G16" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G16" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H16" s="2"/>
@@ -1548,7 +1505,7 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
@@ -1561,14 +1518,14 @@
       <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="6" t="n">
+      <c r="E17" s="5">
         <v>70</v>
       </c>
-      <c r="F17" s="6" t="n">
+      <c r="F17" s="5">
         <v>74</v>
       </c>
-      <c r="G17" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G17" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H17" s="2"/>
@@ -1608,7 +1565,7 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1621,14 +1578,14 @@
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="6" t="n">
+      <c r="E18" s="5">
         <v>75</v>
       </c>
-      <c r="F18" s="6" t="n">
+      <c r="F18" s="5">
         <v>79</v>
       </c>
-      <c r="G18" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G18" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H18" s="2"/>
@@ -1668,7 +1625,7 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1681,14 +1638,14 @@
       <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="6" t="n">
+      <c r="E19" s="5">
         <v>80</v>
       </c>
-      <c r="F19" s="6" t="n">
+      <c r="F19" s="5">
         <v>84</v>
       </c>
-      <c r="G19" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G19" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H19" s="2"/>
@@ -1728,7 +1685,7 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
@@ -1741,14 +1698,14 @@
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="6" t="n">
+      <c r="E20" s="5">
         <v>85</v>
       </c>
-      <c r="F20" s="6" t="n">
+      <c r="F20" s="5">
         <v>999</v>
       </c>
-      <c r="G20" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G20" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H20" s="2"/>
@@ -1788,7 +1745,7 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -1796,19 +1753,19 @@
         <v>44</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="6" t="n">
+      <c r="E21" s="5">
         <v>13</v>
       </c>
-      <c r="F21" s="6" t="n">
+      <c r="F21" s="5">
         <v>17</v>
       </c>
-      <c r="G21" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G21" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H21" s="2"/>
@@ -1846,27 +1803,27 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="6" t="n">
+      <c r="E22" s="5">
         <v>15</v>
       </c>
-      <c r="F22" s="6" t="n">
+      <c r="F22" s="5">
         <v>20</v>
       </c>
-      <c r="G22" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G22" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H22" s="2"/>
@@ -1904,27 +1861,27 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="6" t="n">
+      <c r="E23" s="5">
         <v>15</v>
       </c>
-      <c r="F23" s="6" t="n">
+      <c r="F23" s="5">
         <v>999</v>
       </c>
-      <c r="G23" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G23" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H23" s="2"/>
@@ -1962,27 +1919,27 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="6" t="n">
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
         <v>999</v>
       </c>
-      <c r="G24" s="7" t="b">
-        <f aca="false">TRUE()</f>
+      <c r="G24" s="6" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -2024,7 +1981,7 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -2035,20 +1992,20 @@
         <v>9</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>10</v>
+      </c>
+      <c r="G25" s="6" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E25" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G25" s="7" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2064,7 +2021,7 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -2075,41 +2032,41 @@
         <v>9</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="5">
+        <v>11</v>
+      </c>
+      <c r="F26" s="5">
+        <v>13</v>
+      </c>
+      <c r="G26" s="6" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O26" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E26" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="F26" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="G26" s="7" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -2118,7 +2075,7 @@
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
@@ -2129,52 +2086,52 @@
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E27" s="5">
         <v>14</v>
       </c>
-      <c r="F27" s="6" t="n">
+      <c r="F27" s="5">
         <v>15</v>
       </c>
-      <c r="G27" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G27" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N27" s="2" t="s">
+      <c r="O27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="O27" s="2" t="s">
+      <c r="P27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P27" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="Q27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -2185,50 +2142,50 @@
         <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E28" s="5">
         <v>16</v>
       </c>
-      <c r="F28" s="6" t="n">
+      <c r="F28" s="5">
         <v>17</v>
       </c>
-      <c r="G28" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G28" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="N28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="O28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="O28" s="2" t="s">
+      <c r="P28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="Q28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Q28" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="R28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
@@ -2239,16 +2196,16 @@
         <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E29" s="5">
         <v>18</v>
       </c>
-      <c r="F29" s="6" t="n">
+      <c r="F29" s="5">
         <v>20</v>
       </c>
-      <c r="G29" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G29" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H29" s="2"/>
@@ -2256,37 +2213,37 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="O29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="P29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="Q29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="R29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="S29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S29" s="2" t="s">
+      <c r="T29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T29" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U29" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2297,16 +2254,16 @@
         <v>9</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E30" s="5">
         <v>18</v>
       </c>
-      <c r="F30" s="6" t="n">
+      <c r="F30" s="5">
         <v>23</v>
       </c>
-      <c r="G30" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G30" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H30" s="2"/>
@@ -2314,37 +2271,37 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="N30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="O30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="P30" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="Q30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" s="2" t="s">
+      <c r="R30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R30" s="2" t="s">
+      <c r="S30" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S30" s="2" t="s">
+      <c r="T30" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T30" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U30" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -2355,16 +2312,16 @@
         <v>9</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E31" s="5">
         <v>21</v>
       </c>
-      <c r="F31" s="6" t="n">
+      <c r="F31" s="5">
         <v>99</v>
       </c>
-      <c r="G31" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G31" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H31" s="2"/>
@@ -2372,40 +2329,40 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="N31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="O31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O31" s="2" t="s">
+      <c r="P31" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P31" s="2" t="s">
+      <c r="Q31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="R31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="S31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S31" s="2" t="s">
+      <c r="T31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="U31" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="U31" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="B32" s="2" t="s">
         <v>36</v>
       </c>
@@ -2413,16 +2370,16 @@
         <v>36</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E32" s="5">
         <v>30</v>
       </c>
-      <c r="F32" s="6" t="n">
+      <c r="F32" s="5">
         <v>34</v>
       </c>
-      <c r="G32" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G32" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H32" s="2"/>
@@ -2430,40 +2387,40 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N32" s="2" t="s">
+      <c r="O32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O32" s="2" t="s">
+      <c r="P32" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P32" s="2" t="s">
+      <c r="Q32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q32" s="2" t="s">
+      <c r="R32" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R32" s="2" t="s">
+      <c r="S32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S32" s="2" t="s">
+      <c r="T32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T32" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U32" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="B33" s="2" t="s">
         <v>36</v>
       </c>
@@ -2471,16 +2428,16 @@
         <v>36</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E33" s="5">
         <v>35</v>
       </c>
-      <c r="F33" s="6" t="n">
+      <c r="F33" s="5">
         <v>39</v>
       </c>
-      <c r="G33" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G33" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H33" s="2"/>
@@ -2488,39 +2445,39 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M33" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N33" s="2" t="s">
+      <c r="O33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O33" s="2" t="s">
+      <c r="P33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P33" s="2" t="s">
+      <c r="Q33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q33" s="2" t="s">
+      <c r="R33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R33" s="2" t="s">
+      <c r="S33" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S33" s="2" t="s">
+      <c r="T33" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T33" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U33" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>36</v>
@@ -2529,16 +2486,16 @@
         <v>36</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E34" s="5">
         <v>40</v>
       </c>
-      <c r="F34" s="6" t="n">
+      <c r="F34" s="5">
         <v>44</v>
       </c>
-      <c r="G34" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G34" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H34" s="2"/>
@@ -2546,39 +2503,39 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="N34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="P34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P34" s="2" t="s">
+      <c r="Q34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q34" s="2" t="s">
+      <c r="R34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R34" s="2" t="s">
+      <c r="S34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S34" s="2" t="s">
+      <c r="T34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T34" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U34" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>36</v>
@@ -2587,16 +2544,16 @@
         <v>36</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E35" s="5">
         <v>45</v>
       </c>
-      <c r="F35" s="6" t="n">
+      <c r="F35" s="5">
         <v>49</v>
       </c>
-      <c r="G35" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G35" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H35" s="2"/>
@@ -2604,39 +2561,39 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="N35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="O35" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O35" s="2" t="s">
+      <c r="P35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P35" s="2" t="s">
+      <c r="Q35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q35" s="2" t="s">
+      <c r="R35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R35" s="2" t="s">
+      <c r="S35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S35" s="2" t="s">
+      <c r="T35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T35" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U35" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>36</v>
@@ -2645,16 +2602,16 @@
         <v>36</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="5">
         <v>50</v>
       </c>
-      <c r="E36" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="F36" s="6" t="n">
+      <c r="F36" s="5">
         <v>54</v>
       </c>
-      <c r="G36" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G36" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H36" s="2"/>
@@ -2662,39 +2619,39 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N36" s="2" t="s">
+      <c r="O36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="P36" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P36" s="2" t="s">
+      <c r="Q36" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q36" s="2" t="s">
+      <c r="R36" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R36" s="2" t="s">
+      <c r="S36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S36" s="2" t="s">
+      <c r="T36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T36" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U36" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>36</v>
@@ -2703,16 +2660,16 @@
         <v>36</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E37" s="5">
         <v>55</v>
       </c>
-      <c r="F37" s="6" t="n">
+      <c r="F37" s="5">
         <v>59</v>
       </c>
-      <c r="G37" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G37" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H37" s="2"/>
@@ -2720,39 +2677,39 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="N37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="O37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="P37" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P37" s="2" t="s">
+      <c r="Q37" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q37" s="2" t="s">
+      <c r="R37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R37" s="2" t="s">
+      <c r="S37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S37" s="2" t="s">
+      <c r="T37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T37" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U37" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>36</v>
@@ -2761,16 +2718,16 @@
         <v>36</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E38" s="5">
         <v>60</v>
       </c>
-      <c r="F38" s="6" t="n">
+      <c r="F38" s="5">
         <v>64</v>
       </c>
-      <c r="G38" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G38" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H38" s="2"/>
@@ -2778,39 +2735,39 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M38" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="N38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="O38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="P38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P38" s="2" t="s">
+      <c r="Q38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q38" s="2" t="s">
+      <c r="R38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R38" s="2" t="s">
+      <c r="S38" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S38" s="2" t="s">
+      <c r="T38" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T38" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U38" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>36</v>
@@ -2819,16 +2776,16 @@
         <v>36</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E39" s="5">
         <v>65</v>
       </c>
-      <c r="F39" s="6" t="n">
+      <c r="F39" s="5">
         <v>69</v>
       </c>
-      <c r="G39" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G39" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H39" s="2"/>
@@ -2836,57 +2793,57 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M39" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="N39" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="O39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="P39" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P39" s="2" t="s">
+      <c r="Q39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q39" s="2" t="s">
+      <c r="R39" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R39" s="2" t="s">
+      <c r="S39" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S39" s="2" t="s">
+      <c r="T39" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T39" s="2" t="s">
+      <c r="U39" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="5">
         <v>70</v>
       </c>
-      <c r="U39" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="F40" s="5">
         <v>74</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="6" t="n">
-        <v>70</v>
-      </c>
-      <c r="F40" s="6" t="n">
-        <v>74</v>
-      </c>
-      <c r="G40" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G40" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H40" s="2"/>
@@ -2894,57 +2851,57 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="N40" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N40" s="2" t="s">
+      <c r="O40" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="P40" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P40" s="2" t="s">
+      <c r="Q40" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q40" s="2" t="s">
+      <c r="R40" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R40" s="2" t="s">
+      <c r="S40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S40" s="2" t="s">
+      <c r="T40" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T40" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U40" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="5">
         <v>75</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="6" t="n">
-        <v>75</v>
-      </c>
-      <c r="F41" s="6" t="n">
+      <c r="F41" s="5">
         <v>79</v>
       </c>
-      <c r="G41" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G41" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H41" s="2"/>
@@ -2952,39 +2909,39 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M41" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M41" s="2" t="s">
+      <c r="N41" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N41" s="2" t="s">
+      <c r="O41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O41" s="2" t="s">
+      <c r="P41" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P41" s="2" t="s">
+      <c r="Q41" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q41" s="2" t="s">
+      <c r="R41" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R41" s="2" t="s">
+      <c r="S41" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S41" s="2" t="s">
+      <c r="T41" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T41" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U41" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>36</v>
@@ -2993,16 +2950,16 @@
         <v>36</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E42" s="5">
         <v>80</v>
       </c>
-      <c r="F42" s="6" t="n">
+      <c r="F42" s="5">
         <v>84</v>
       </c>
-      <c r="G42" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G42" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H42" s="2"/>
@@ -3010,39 +2967,39 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M42" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O42" s="2" t="s">
+      <c r="P42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P42" s="2" t="s">
+      <c r="Q42" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q42" s="2" t="s">
+      <c r="R42" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R42" s="2" t="s">
+      <c r="S42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S42" s="2" t="s">
+      <c r="T42" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T42" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U42" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>36</v>
@@ -3051,16 +3008,16 @@
         <v>36</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E43" s="5">
         <v>85</v>
       </c>
-      <c r="F43" s="6" t="n">
+      <c r="F43" s="5">
         <v>999</v>
       </c>
-      <c r="G43" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G43" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H43" s="2"/>
@@ -3068,37 +3025,37 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M43" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M43" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N43" s="2" t="s">
+      <c r="O43" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O43" s="2" t="s">
+      <c r="P43" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P43" s="2" t="s">
+      <c r="Q43" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q43" s="2" t="s">
+      <c r="R43" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R43" s="2" t="s">
+      <c r="S43" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S43" s="2" t="s">
+      <c r="T43" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T43" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U43" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -3106,77 +3063,77 @@
         <v>44</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E44" s="5">
         <v>13</v>
       </c>
-      <c r="F44" s="6" t="n">
+      <c r="F44" s="5">
         <v>17</v>
       </c>
-      <c r="G44" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G44" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L44" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M44" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M44" s="2" t="s">
+      <c r="N44" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="O44" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O44" s="2" t="s">
+      <c r="P44" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P44" s="2" t="s">
+      <c r="Q44" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q44" s="2" t="s">
+      <c r="R44" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R44" s="2" t="s">
+      <c r="S44" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S44" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="T44" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E45" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E45" s="5">
         <v>15</v>
       </c>
-      <c r="F45" s="6" t="n">
+      <c r="F45" s="5">
         <v>20</v>
       </c>
-      <c r="G45" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G45" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H45" s="2"/>
@@ -3184,57 +3141,57 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M45" s="2" t="s">
+      <c r="N45" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N45" s="2" t="s">
+      <c r="O45" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O45" s="2" t="s">
+      <c r="P45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P45" s="2" t="s">
+      <c r="Q45" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q45" s="2" t="s">
+      <c r="R45" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R45" s="2" t="s">
+      <c r="S45" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S45" s="2" t="s">
+      <c r="T45" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T45" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U45" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E46" s="5">
         <v>15</v>
       </c>
-      <c r="F46" s="6" t="n">
+      <c r="F46" s="5">
         <v>999</v>
       </c>
-      <c r="G46" s="7" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="G46" s="6" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H46" s="2"/>
@@ -3242,112 +3199,107 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M46" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="N46" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="O46" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O46" s="2" t="s">
+      <c r="P46" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P46" s="2" t="s">
+      <c r="Q46" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q46" s="2" t="s">
+      <c r="R46" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R46" s="2" t="s">
+      <c r="S46" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S46" s="2" t="s">
+      <c r="T46" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T46" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="U46" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="5">
+        <v>0</v>
+      </c>
+      <c r="F47" s="5">
+        <v>999</v>
+      </c>
+      <c r="G47" s="6" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="I47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U47" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E47" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="6" t="n">
-        <v>999</v>
-      </c>
-      <c r="G47" s="7" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N47" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="S47" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T47" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="U47" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H1:J1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "removed championship type IWF as it doesn't matter."
This reverts commit c3d8ae6a8329f361ef295ba37e237b23b8513f2f.
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/DE-AgeGroups_de.xlsx
+++ b/owlcms/src/main/resources/agegroups/DE-AgeGroups_de.xlsx
@@ -1,31 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABEE59E-AEEF-4A46-8101-01C4A6EB49C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2925" windowWidth="23985" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BW vs AgeGroups" sheetId="1" r:id="rId1"/>
+    <sheet name="BW vs AgeGroups" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -34,267 +20,293 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="77">
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>championship Name</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>#bodyweight categories or each age group (bodyweight category code followed by optional qualifying total, example: 45 80)</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>F999</t>
-  </si>
-  <si>
-    <t>U13</t>
-  </si>
-  <si>
-    <t>F40</t>
-  </si>
-  <si>
-    <t>F44</t>
-  </si>
-  <si>
-    <t>F48</t>
-  </si>
-  <si>
-    <t>F53</t>
-  </si>
-  <si>
-    <t>F58</t>
-  </si>
-  <si>
-    <t>F63</t>
-  </si>
-  <si>
-    <t>U15</t>
-  </si>
-  <si>
-    <t>U17</t>
-  </si>
-  <si>
-    <t>F69</t>
-  </si>
-  <si>
-    <t>F75</t>
-  </si>
-  <si>
-    <t>U20</t>
-  </si>
-  <si>
-    <t>F45</t>
-  </si>
-  <si>
-    <t>F49</t>
-  </si>
-  <si>
-    <t>F55</t>
-  </si>
-  <si>
-    <t>F59</t>
-  </si>
-  <si>
-    <t>F64</t>
-  </si>
-  <si>
-    <t>F71</t>
-  </si>
-  <si>
-    <t>F76</t>
-  </si>
-  <si>
-    <t>F81</t>
-  </si>
-  <si>
-    <t>F87</t>
-  </si>
-  <si>
-    <t>U23</t>
-  </si>
-  <si>
-    <t>O21</t>
-  </si>
-  <si>
-    <t>F30</t>
-  </si>
-  <si>
-    <t>MASTERS</t>
-  </si>
-  <si>
-    <t>F35</t>
-  </si>
-  <si>
-    <t>F50</t>
-  </si>
-  <si>
-    <t>F60</t>
-  </si>
-  <si>
-    <t>F65</t>
-  </si>
-  <si>
-    <t>F70</t>
-  </si>
-  <si>
-    <t>F80</t>
-  </si>
-  <si>
-    <t>F85</t>
-  </si>
-  <si>
-    <t>YTH</t>
-  </si>
-  <si>
-    <t>JR</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>DEFAULT</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>M999</t>
-  </si>
-  <si>
-    <t>M35</t>
-  </si>
-  <si>
-    <t>M40</t>
-  </si>
-  <si>
-    <t>M45</t>
-  </si>
-  <si>
-    <t>M50</t>
-  </si>
-  <si>
-    <t>M56</t>
-  </si>
-  <si>
-    <t>M62</t>
-  </si>
-  <si>
-    <t>M69</t>
-  </si>
-  <si>
-    <t>M77</t>
-  </si>
-  <si>
-    <t>M85</t>
-  </si>
-  <si>
-    <t>M94</t>
-  </si>
-  <si>
-    <t>M55</t>
-  </si>
-  <si>
-    <t>M61</t>
-  </si>
-  <si>
-    <t>M67</t>
-  </si>
-  <si>
-    <t>M73</t>
-  </si>
-  <si>
-    <t>M81</t>
-  </si>
-  <si>
-    <t>M89</t>
-  </si>
-  <si>
-    <t>M96</t>
-  </si>
-  <si>
-    <t>M102</t>
-  </si>
-  <si>
-    <t>M109</t>
-  </si>
-  <si>
-    <t>M30</t>
-  </si>
-  <si>
-    <t>M60</t>
-  </si>
-  <si>
-    <t>M65</t>
-  </si>
-  <si>
-    <t>M70</t>
-  </si>
-  <si>
-    <t>M75</t>
-  </si>
-  <si>
-    <t>M80</t>
-  </si>
-  <si>
-    <t>M49</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="78">
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">championship Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#bodyweight categories or each age group (bodyweight category code followed by optional qualifying total, example: 45 80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MASTERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IWF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFAULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -313,7 +325,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -321,27 +333,73 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+  <cellXfs count="8">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -400,76 +458,60 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="44546a"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="e7e6e6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="5b9bd5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="ed7d31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="a5a5a5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="ffc000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4472c4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="70ad47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0563c1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="954f72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -501,7 +543,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -525,7 +567,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -585,30 +627,31 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -630,24 +673,24 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-    </row>
-    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -660,14 +703,14 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="E2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G2" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -687,7 +730,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -700,14 +743,14 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="G3" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G3" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H3" s="2"/>
@@ -739,7 +782,7 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
     </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -752,14 +795,14 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="G4" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G4" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H4" s="2"/>
@@ -791,7 +834,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -804,14 +847,14 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="G5" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G5" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H5" s="2"/>
@@ -845,7 +888,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -858,14 +901,14 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="G6" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G6" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H6" s="2"/>
@@ -905,7 +948,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -918,14 +961,14 @@
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="G7" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G7" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="2"/>
@@ -965,7 +1008,7 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -978,14 +1021,14 @@
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6" t="n">
         <v>999</v>
       </c>
-      <c r="G8" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G8" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H8" s="2"/>
@@ -1025,7 +1068,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1038,14 +1081,14 @@
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="G9" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G9" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H9" s="2"/>
@@ -1085,7 +1128,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -1098,14 +1141,14 @@
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="6" t="n">
         <v>35</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="G10" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G10" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H10" s="2"/>
@@ -1145,7 +1188,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1158,14 +1201,14 @@
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="G11" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G11" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H11" s="2"/>
@@ -1205,7 +1248,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1218,14 +1261,14 @@
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6" t="n">
         <v>49</v>
       </c>
-      <c r="G12" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G12" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H12" s="2"/>
@@ -1265,7 +1308,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1278,14 +1321,14 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="6" t="n">
         <v>54</v>
       </c>
-      <c r="G13" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G13" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H13" s="2"/>
@@ -1325,7 +1368,7 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1338,14 +1381,14 @@
       <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="6" t="n">
         <v>55</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="G14" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G14" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H14" s="2"/>
@@ -1385,7 +1428,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1398,14 +1441,14 @@
       <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6" t="n">
         <v>60</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6" t="n">
         <v>64</v>
       </c>
-      <c r="G15" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G15" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H15" s="2"/>
@@ -1445,7 +1488,7 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1458,14 +1501,14 @@
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6" t="n">
         <v>69</v>
       </c>
-      <c r="G16" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G16" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H16" s="2"/>
@@ -1505,7 +1548,7 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
@@ -1518,14 +1561,14 @@
       <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="6" t="n">
         <v>70</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="6" t="n">
         <v>74</v>
       </c>
-      <c r="G17" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G17" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H17" s="2"/>
@@ -1565,7 +1608,7 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1578,14 +1621,14 @@
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="6" t="n">
         <v>79</v>
       </c>
-      <c r="G18" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G18" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H18" s="2"/>
@@ -1625,7 +1668,7 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
-    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1638,14 +1681,14 @@
       <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="6" t="n">
         <v>80</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="6" t="n">
         <v>84</v>
       </c>
-      <c r="G19" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G19" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H19" s="2"/>
@@ -1685,7 +1728,7 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
     </row>
-    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
@@ -1698,14 +1741,14 @@
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="6" t="n">
         <v>85</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="6" t="n">
         <v>999</v>
       </c>
-      <c r="G20" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G20" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H20" s="2"/>
@@ -1745,7 +1788,7 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -1753,19 +1796,19 @@
         <v>44</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="G21" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G21" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H21" s="2"/>
@@ -1803,27 +1846,27 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
     </row>
-    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="G22" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G22" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H22" s="2"/>
@@ -1861,27 +1904,27 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="6" t="n">
         <v>999</v>
       </c>
-      <c r="G23" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G23" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H23" s="2"/>
@@ -1919,27 +1962,27 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5">
+      <c r="E24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6" t="n">
         <v>999</v>
       </c>
-      <c r="G24" s="6" t="b">
-        <f>TRUE()</f>
+      <c r="G24" s="7" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -1981,7 +2024,7 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
     </row>
-    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1992,20 +2035,20 @@
         <v>9</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
+        <v>50</v>
+      </c>
+      <c r="E25" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="G25" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G25" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2021,7 +2064,7 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
     </row>
-    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -2032,41 +2075,41 @@
         <v>9</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="5">
+        <v>50</v>
+      </c>
+      <c r="E26" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="G26" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G26" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O26" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -2075,7 +2118,7 @@
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
     </row>
-    <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
@@ -2086,52 +2129,52 @@
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="5">
+        <v>50</v>
+      </c>
+      <c r="E27" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="G27" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G27" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
     </row>
-    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -2142,50 +2185,50 @@
         <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="5">
+        <v>50</v>
+      </c>
+      <c r="E28" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="G28" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G28" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
@@ -2196,16 +2239,16 @@
         <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="5">
+        <v>50</v>
+      </c>
+      <c r="E29" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="G29" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G29" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H29" s="2"/>
@@ -2213,37 +2256,37 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2254,16 +2297,16 @@
         <v>9</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="5">
+        <v>50</v>
+      </c>
+      <c r="E30" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="G30" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G30" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H30" s="2"/>
@@ -2271,37 +2314,37 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -2312,16 +2355,16 @@
         <v>9</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="5">
+        <v>50</v>
+      </c>
+      <c r="E31" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="6" t="n">
         <v>99</v>
       </c>
-      <c r="G31" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G31" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H31" s="2"/>
@@ -2329,57 +2372,57 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U31" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="5">
+      <c r="E32" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="G32" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G32" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H32" s="2"/>
@@ -2387,57 +2430,57 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U32" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="5">
+      <c r="E33" s="6" t="n">
         <v>35</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="G33" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G33" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H33" s="2"/>
@@ -2445,57 +2488,57 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U33" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="5">
+      <c r="E34" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="G34" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G34" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H34" s="2"/>
@@ -2503,57 +2546,57 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U34" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="F35" s="6" t="n">
         <v>49</v>
       </c>
-      <c r="E35" s="5">
-        <v>45</v>
-      </c>
-      <c r="F35" s="5">
-        <v>49</v>
-      </c>
-      <c r="G35" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G35" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H35" s="2"/>
@@ -2561,57 +2604,57 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U35" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="E36" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F36" s="6" t="n">
         <v>54</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="5">
-        <v>50</v>
-      </c>
-      <c r="F36" s="5">
-        <v>54</v>
-      </c>
-      <c r="G36" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G36" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H36" s="2"/>
@@ -2619,57 +2662,57 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U36" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N36" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U36" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="5">
+      <c r="E37" s="6" t="n">
         <v>55</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="G37" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G37" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H37" s="2"/>
@@ -2677,57 +2720,57 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="F38" s="6" t="n">
         <v>64</v>
       </c>
-      <c r="P37" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U37" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="5">
-        <v>60</v>
-      </c>
-      <c r="F38" s="5">
-        <v>64</v>
-      </c>
-      <c r="G38" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G38" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H38" s="2"/>
@@ -2735,57 +2778,57 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U38" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="Q38" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T38" s="2" t="s">
+      <c r="F39" s="6" t="n">
         <v>69</v>
       </c>
-      <c r="U38" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="5">
-        <v>65</v>
-      </c>
-      <c r="F39" s="5">
-        <v>69</v>
-      </c>
-      <c r="G39" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G39" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H39" s="2"/>
@@ -2793,57 +2836,57 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U39" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="5">
+      <c r="E40" s="6" t="n">
         <v>70</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="6" t="n">
         <v>74</v>
       </c>
-      <c r="G40" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G40" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H40" s="2"/>
@@ -2851,57 +2894,57 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U40" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E41" s="5">
+      <c r="E41" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="6" t="n">
         <v>79</v>
       </c>
-      <c r="G41" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G41" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H41" s="2"/>
@@ -2909,57 +2952,57 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U41" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E42" s="5">
+      <c r="E42" s="6" t="n">
         <v>80</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="6" t="n">
         <v>84</v>
       </c>
-      <c r="G42" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G42" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H42" s="2"/>
@@ -2967,57 +3010,57 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U42" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="5">
+      <c r="E43" s="6" t="n">
         <v>85</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="6" t="n">
         <v>999</v>
       </c>
-      <c r="G43" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G43" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H43" s="2"/>
@@ -3025,37 +3068,37 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U43" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -3063,77 +3106,77 @@
         <v>44</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="5">
+        <v>50</v>
+      </c>
+      <c r="E44" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="G44" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G44" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T44" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="U44" s="2"/>
-    </row>
-    <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45" s="5">
+      <c r="E45" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="G45" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G45" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H45" s="2"/>
@@ -3141,57 +3184,57 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U45" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E46" s="5">
+      <c r="E46" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="6" t="n">
         <v>999</v>
       </c>
-      <c r="G46" s="6" t="b">
-        <f>FALSE()</f>
+      <c r="G46" s="7" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H46" s="2"/>
@@ -3199,107 +3242,112 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U46" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="6" t="n">
+        <v>999</v>
+      </c>
+      <c r="G47" s="7" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="M47" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O46" s="2" t="s">
+      <c r="N47" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P46" s="2" t="s">
+      <c r="O47" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q46" s="2" t="s">
+      <c r="P47" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="R46" s="2" t="s">
+      <c r="Q47" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="S46" s="2" t="s">
+      <c r="R47" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="T46" s="2" t="s">
+      <c r="S47" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U46" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="5">
-        <v>0</v>
-      </c>
-      <c r="F47" s="5">
-        <v>999</v>
-      </c>
-      <c r="G47" s="6" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H47" s="2" t="s">
+      <c r="T47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U47" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N47" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S47" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T47" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U47" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H1:J1"/>
   </mergeCells>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>